<commit_message>
Added get related data objects from sparql endpoint functionality to RdfProjectionEngine.
</commit_message>
<xml_diff>
--- a/iRINGTools.ESB/documents/Review&AcceptanceGridDesign2.xlsx
+++ b/iRINGTools.ESB/documents/Review&AcceptanceGridDesign2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="17235" windowHeight="11310" tabRatio="867" activeTab="5"/>
+    <workbookView xWindow="360" yWindow="45" windowWidth="17235" windowHeight="11310" tabRatio="867" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tree" sheetId="5" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="77">
   <si>
     <t>IdentificationByTag</t>
   </si>
@@ -251,6 +251,9 @@
   </si>
   <si>
     <t>1. There's only one row with the current sample DXO; will be many when individual related to parent as 1 to many</t>
+  </si>
+  <si>
+    <t>FluidComp-1</t>
   </si>
 </sst>
 </file>
@@ -311,14 +314,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -331,21 +333,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -643,8 +647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74:XFD74"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -722,8 +726,8 @@
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="F15" t="s">
-        <v>44</v>
+      <c r="F15" s="12" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="2:6">
@@ -922,22 +926,22 @@
       </c>
     </row>
     <row r="62" spans="1:6">
-      <c r="A62" s="12" t="s">
+      <c r="A62" s="11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="63" spans="1:6" s="18" customFormat="1">
-      <c r="A63" s="18" t="s">
+    <row r="63" spans="1:6" s="19" customFormat="1">
+      <c r="A63" s="19" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="64" spans="1:6" s="7" customFormat="1">
-      <c r="A64" s="7" t="s">
+    <row r="64" spans="1:6" s="17" customFormat="1">
+      <c r="A64" s="17" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="65" spans="1:1" s="13" customFormat="1">
-      <c r="A65" s="13" t="s">
+    <row r="65" spans="1:1" s="18" customFormat="1">
+      <c r="A65" s="18" t="s">
         <v>41</v>
       </c>
     </row>
@@ -966,8 +970,8 @@
         <v>65</v>
       </c>
     </row>
-    <row r="71" spans="1:1" s="13" customFormat="1">
-      <c r="A71" s="13" t="s">
+    <row r="71" spans="1:1" s="18" customFormat="1">
+      <c r="A71" s="18" t="s">
         <v>68</v>
       </c>
     </row>
@@ -981,8 +985,8 @@
         <v>74</v>
       </c>
     </row>
-    <row r="74" spans="1:1" s="13" customFormat="1">
-      <c r="A74" s="13" t="s">
+    <row r="74" spans="1:1" s="18" customFormat="1">
+      <c r="A74" s="18" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1138,25 +1142,25 @@
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="11" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="8" customFormat="1">
-      <c r="A16" s="14"/>
-    </row>
-    <row r="17" spans="1:1" s="15" customFormat="1">
-      <c r="A17" s="15" t="s">
+    <row r="16" spans="1:5" s="7" customFormat="1">
+      <c r="A16" s="13"/>
+    </row>
+    <row r="17" spans="1:1" s="20" customFormat="1">
+      <c r="A17" s="20" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:1" s="13" customFormat="1">
-      <c r="A18" s="13" t="s">
+    <row r="18" spans="1:1" s="18" customFormat="1">
+      <c r="A18" s="18" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:1" s="13" customFormat="1">
-      <c r="A19" s="13" t="s">
+    <row r="19" spans="1:1" s="18" customFormat="1">
+      <c r="A19" s="18" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1175,8 +1179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1196,59 +1200,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="10" t="s">
-        <v>1</v>
+      <c r="A1" s="9" t="s">
+        <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="8"/>
-      <c r="B6" s="9"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="8"/>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="8"/>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="8"/>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="11" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1257,11 +1261,11 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:2" s="16" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A12" s="17" t="s">
+    <row r="12" spans="1:2" s="14" customFormat="1" ht="33.75" customHeight="1">
+      <c r="A12" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="B12" s="17"/>
+      <c r="B12" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1295,7 +1299,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:1" s="13" customFormat="1"/>
+    <row r="10" spans="1:1" s="18" customFormat="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A10:XFD10"/>
@@ -1336,7 +1340,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -1366,8 +1370,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="13" customFormat="1">
-      <c r="A11" s="13" t="s">
+    <row r="11" spans="1:2" s="18" customFormat="1">
+      <c r="A11" s="18" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1440,13 +1444,13 @@
       <c r="A2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="19">
+      <c r="B2" s="15">
         <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="20">
+      <c r="D2" s="16">
         <v>1</v>
       </c>
     </row>
@@ -1474,7 +1478,7 @@
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="16" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>